<commit_message>
turn back on covid recession
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junshepard/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/NM/ctrl-settings/GDPGR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\New Mexico\New_Mexico-EPS\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C952D9-6C86-F145-8F9A-4A84F12A553C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66760BB-F573-49E2-A09E-C68C71DBAA73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1380" windowWidth="18520" windowHeight="14040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="585" windowWidth="15675" windowHeight="11355" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -601,12 +601,12 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -614,12 +614,12 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -627,174 +627,174 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -816,15 +816,15 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="7" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="7" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
@@ -838,7 +838,7 @@
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2019</v>
       </c>
@@ -855,7 +855,7 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>51</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -892,7 +892,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>41</v>
       </c>
@@ -935,7 +935,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
@@ -946,7 +946,7 @@
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="12"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -955,7 +955,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -982,7 +982,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
     </row>
-    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1035,15 +1035,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -1051,12 +1051,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="22">
-        <v>0.02</v>
+        <f>Data!B14</f>
+        <v>-3.5040854808296662E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1073,12 +1074,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>

</xml_diff>